<commit_message>
Update Professional Skills Matrix.xlsx
</commit_message>
<xml_diff>
--- a/SSD/Professional Skills Matrix.xlsx
+++ b/SSD/Professional Skills Matrix.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael Botha\Documents\GitHub\ePortfolio-MSc\OOIS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael Botha\Documents\GitHub\ePortfolio-MSc\SSD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0C305D1-BC3E-4C28-9381-5F8184565CFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E4C4643-6273-4BF3-8495-4339DBEAB87F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F0AC6F20-2752-4433-AA8C-078D6A73E621}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="76">
   <si>
     <t>Competency</t>
   </si>
@@ -237,10 +237,6 @@
   </si>
   <si>
     <t>Adapted from BCS guidelines and Essex graduate</t>
-  </si>
-  <si>
-    <t>&gt; Pearson Language test
-&gt; Liaison with various parties</t>
   </si>
   <si>
     <t xml:space="preserve">&gt; PoE </t>
@@ -267,10 +263,20 @@
     </r>
   </si>
   <si>
-    <t>&gt; 11 years in team envirnoment</t>
-  </si>
-  <si>
-    <t>&gt; Working in critical services environment</t>
+    <t>&gt; Pearson Language test
+&gt; Liaison with various parties
+&gt; PoE</t>
+  </si>
+  <si>
+    <t>&gt; PoE 
+&gt; OneNote Notebooks</t>
+  </si>
+  <si>
+    <t>&gt; Worked in critical services environment</t>
+  </si>
+  <si>
+    <t>&gt; 11 years in team envirnoment
+&gt; PoE</t>
   </si>
 </sst>
 </file>
@@ -493,6 +499,8 @@
       <alignment horizontal="left" vertical="center" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -529,8 +537,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -847,8 +853,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E859C549-79C4-4FD7-AE1D-68AD30B27DE0}">
   <dimension ref="A1:I42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -878,16 +884,16 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="25" t="s">
+      <c r="H1" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="25"/>
-    </row>
-    <row r="2" spans="1:9" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="20" t="s">
+      <c r="I1" s="27"/>
+    </row>
+    <row r="2" spans="1:9" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="25" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="3" t="s">
@@ -897,7 +903,7 @@
         <v>16</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="H2" s="4" t="s">
         <v>9</v>
@@ -907,8 +913,8 @@
       </c>
     </row>
     <row r="3" spans="1:9" s="2" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="20"/>
-      <c r="B3" s="24"/>
+      <c r="A3" s="22"/>
+      <c r="B3" s="26"/>
       <c r="C3" s="5" t="s">
         <v>11</v>
       </c>
@@ -916,7 +922,7 @@
         <v>16</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H3" s="4" t="s">
         <v>12</v>
@@ -926,8 +932,8 @@
       </c>
     </row>
     <row r="4" spans="1:9" s="2" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="20"/>
-      <c r="B4" s="22" t="s">
+      <c r="A4" s="22"/>
+      <c r="B4" s="24" t="s">
         <v>14</v>
       </c>
       <c r="C4" s="3" t="s">
@@ -937,7 +943,7 @@
         <v>12</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="H4" s="4" t="s">
         <v>16</v>
@@ -947,8 +953,8 @@
       </c>
     </row>
     <row r="5" spans="1:9" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="20"/>
-      <c r="B5" s="23"/>
+      <c r="A5" s="22"/>
+      <c r="B5" s="25"/>
       <c r="C5" s="6" t="s">
         <v>18</v>
       </c>
@@ -956,7 +962,7 @@
         <v>9</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H5" s="4" t="s">
         <v>19</v>
@@ -966,8 +972,8 @@
       </c>
     </row>
     <row r="6" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="20"/>
-      <c r="B6" s="23"/>
+      <c r="A6" s="22"/>
+      <c r="B6" s="25"/>
       <c r="C6" s="6" t="s">
         <v>21</v>
       </c>
@@ -977,21 +983,21 @@
       <c r="E6" s="6"/>
     </row>
     <row r="7" spans="1:9" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="20"/>
-      <c r="B7" s="23"/>
+      <c r="A7" s="22"/>
+      <c r="B7" s="25"/>
       <c r="C7" s="6" t="s">
         <v>22</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:9" s="2" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="20"/>
-      <c r="B8" s="24"/>
+      <c r="A8" s="22"/>
+      <c r="B8" s="26"/>
       <c r="C8" s="5" t="s">
         <v>23</v>
       </c>
@@ -999,27 +1005,27 @@
         <v>9</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="20"/>
-      <c r="B9" s="22" t="s">
+      <c r="A9" s="22"/>
+      <c r="B9" s="24" t="s">
         <v>24</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>25</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E9" s="31" t="s">
-        <v>69</v>
+        <v>16</v>
+      </c>
+      <c r="E9" s="19" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="20"/>
-      <c r="B10" s="23"/>
+      <c r="A10" s="22"/>
+      <c r="B10" s="25"/>
       <c r="C10" s="6" t="s">
         <v>26</v>
       </c>
@@ -1027,27 +1033,27 @@
         <v>16</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="20"/>
-      <c r="B11" s="24"/>
+      <c r="A11" s="22"/>
+      <c r="B11" s="26"/>
       <c r="C11" s="5" t="s">
         <v>27</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E11" s="32" t="s">
-        <v>69</v>
+        <v>16</v>
+      </c>
+      <c r="E11" s="20" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="12" spans="1:9" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="26" t="s">
+      <c r="A12" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="22" t="s">
+      <c r="B12" s="24" t="s">
         <v>29</v>
       </c>
       <c r="C12" s="3" t="s">
@@ -1059,8 +1065,8 @@
       <c r="E12" s="3"/>
     </row>
     <row r="13" spans="1:9" s="2" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="27"/>
-      <c r="B13" s="23"/>
+      <c r="A13" s="29"/>
+      <c r="B13" s="25"/>
       <c r="C13" s="6" t="s">
         <v>31</v>
       </c>
@@ -1070,7 +1076,7 @@
       <c r="E13" s="6"/>
     </row>
     <row r="14" spans="1:9" s="2" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="26" t="s">
+      <c r="A14" s="28" t="s">
         <v>32</v>
       </c>
       <c r="B14" s="12" t="s">
@@ -1080,15 +1086,15 @@
         <v>34</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="15" spans="1:9" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="27"/>
-      <c r="B15" s="22" t="s">
+    <row r="15" spans="1:9" s="2" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="29"/>
+      <c r="B15" s="24" t="s">
         <v>35</v>
       </c>
       <c r="C15" s="3" t="s">
@@ -1098,12 +1104,12 @@
         <v>16</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" s="2" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="27"/>
-      <c r="B16" s="23"/>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" s="2" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="29"/>
+      <c r="B16" s="25"/>
       <c r="C16" s="6" t="s">
         <v>37</v>
       </c>
@@ -1111,12 +1117,12 @@
         <v>16</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" s="2" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="27"/>
-      <c r="B17" s="23"/>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" s="2" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="29"/>
+      <c r="B17" s="25"/>
       <c r="C17" s="6" t="s">
         <v>38</v>
       </c>
@@ -1124,12 +1130,12 @@
         <v>16</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" s="2" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="27"/>
-      <c r="B18" s="24"/>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" s="2" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="29"/>
+      <c r="B18" s="26"/>
       <c r="C18" s="6" t="s">
         <v>39</v>
       </c>
@@ -1137,12 +1143,12 @@
         <v>16</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="19" spans="1:5" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="27"/>
-      <c r="B19" s="28" t="s">
+      <c r="A19" s="29"/>
+      <c r="B19" s="30" t="s">
         <v>40</v>
       </c>
       <c r="C19" s="3" t="s">
@@ -1154,21 +1160,21 @@
       <c r="E19" s="3"/>
     </row>
     <row r="20" spans="1:5" s="2" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="27"/>
-      <c r="B20" s="29"/>
+      <c r="A20" s="29"/>
+      <c r="B20" s="31"/>
       <c r="C20" s="5" t="s">
         <v>42</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E20" s="5"/>
     </row>
     <row r="21" spans="1:5" s="2" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="19" t="s">
+      <c r="A21" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="B21" s="28" t="s">
+      <c r="B21" s="30" t="s">
         <v>44</v>
       </c>
       <c r="C21" s="13" t="s">
@@ -1178,34 +1184,34 @@
       <c r="E21" s="6"/>
     </row>
     <row r="22" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="20"/>
-      <c r="B22" s="30"/>
+      <c r="A22" s="22"/>
+      <c r="B22" s="32"/>
       <c r="C22" s="6" t="s">
         <v>46</v>
       </c>
       <c r="D22" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="E22" s="32" t="s">
-        <v>69</v>
+        <v>16</v>
+      </c>
+      <c r="E22" s="20" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="20"/>
-      <c r="B23" s="30"/>
+      <c r="A23" s="22"/>
+      <c r="B23" s="32"/>
       <c r="C23" s="6" t="s">
         <v>47</v>
       </c>
       <c r="D23" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="E23" s="32" t="s">
-        <v>69</v>
+        <v>16</v>
+      </c>
+      <c r="E23" s="20" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="20"/>
-      <c r="B24" s="30"/>
+      <c r="A24" s="22"/>
+      <c r="B24" s="32"/>
       <c r="C24" s="15" t="s">
         <v>48</v>
       </c>
@@ -1213,47 +1219,47 @@
       <c r="E24" s="14"/>
     </row>
     <row r="25" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="20"/>
-      <c r="B25" s="30"/>
+      <c r="A25" s="22"/>
+      <c r="B25" s="32"/>
       <c r="C25" s="15" t="s">
         <v>49</v>
       </c>
       <c r="D25" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="E25" s="32" t="s">
-        <v>69</v>
+        <v>16</v>
+      </c>
+      <c r="E25" s="20" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="20"/>
-      <c r="B26" s="30"/>
+      <c r="A26" s="22"/>
+      <c r="B26" s="32"/>
       <c r="C26" s="15" t="s">
         <v>50</v>
       </c>
       <c r="D26" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="E26" s="32" t="s">
-        <v>69</v>
+      <c r="E26" s="20" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="20"/>
-      <c r="B27" s="30"/>
+      <c r="A27" s="22"/>
+      <c r="B27" s="32"/>
       <c r="C27" s="6" t="s">
         <v>51</v>
       </c>
       <c r="D27" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="E27" s="32" t="s">
-        <v>69</v>
+      <c r="E27" s="20" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="20"/>
-      <c r="B28" s="30"/>
+      <c r="A28" s="22"/>
+      <c r="B28" s="32"/>
       <c r="C28" s="6" t="s">
         <v>52</v>
       </c>
@@ -1261,62 +1267,62 @@
       <c r="E28" s="14"/>
     </row>
     <row r="29" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="20"/>
-      <c r="B29" s="30"/>
+      <c r="A29" s="22"/>
+      <c r="B29" s="32"/>
       <c r="C29" s="6" t="s">
         <v>53</v>
       </c>
       <c r="D29" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="E29" s="32" t="s">
-        <v>69</v>
+      <c r="E29" s="20" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="20"/>
-      <c r="B30" s="30"/>
+      <c r="A30" s="22"/>
+      <c r="B30" s="32"/>
       <c r="C30" s="6" t="s">
         <v>54</v>
       </c>
       <c r="D30" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="E30" s="32" t="s">
-        <v>69</v>
+      <c r="E30" s="20" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="20"/>
-      <c r="B31" s="30"/>
+      <c r="A31" s="22"/>
+      <c r="B31" s="32"/>
       <c r="C31" s="6" t="s">
         <v>55</v>
       </c>
       <c r="D31" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="E31" s="32" t="s">
-        <v>69</v>
+      <c r="E31" s="20" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="20"/>
-      <c r="B32" s="30"/>
+      <c r="A32" s="22"/>
+      <c r="B32" s="32"/>
       <c r="C32" s="5" t="s">
         <v>56</v>
       </c>
       <c r="D32" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="E32" s="32" t="s">
-        <v>69</v>
+        <v>16</v>
+      </c>
+      <c r="E32" s="20" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="19" t="s">
+      <c r="A33" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="B33" s="22" t="s">
+      <c r="B33" s="24" t="s">
         <v>58</v>
       </c>
       <c r="C33" s="3" t="s">
@@ -1328,8 +1334,8 @@
       <c r="E33" s="7"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="20"/>
-      <c r="B34" s="23"/>
+      <c r="A34" s="22"/>
+      <c r="B34" s="25"/>
       <c r="C34" s="6" t="s">
         <v>60</v>
       </c>
@@ -1339,8 +1345,8 @@
       <c r="E34" s="8"/>
     </row>
     <row r="35" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="20"/>
-      <c r="B35" s="24"/>
+      <c r="A35" s="22"/>
+      <c r="B35" s="26"/>
       <c r="C35" s="5" t="s">
         <v>61</v>
       </c>
@@ -1350,7 +1356,7 @@
       <c r="E35" s="9"/>
     </row>
     <row r="36" spans="1:5" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="21"/>
+      <c r="A36" s="23"/>
       <c r="B36" s="16" t="s">
         <v>62</v>
       </c>

</xml_diff>